<commit_message>
com calculos de media e desvio padrao
</commit_message>
<xml_diff>
--- a/421.xlsx
+++ b/421.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimih\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tqsco\Downloads\MULT_TP2-main (3)\MULT_TP2-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D0D0FB-E378-45D2-91A4-67B3F14CD538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EDAC39-2A8C-4FFE-AE1C-2C08B60F1172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{32CBE812-E37C-4690-A61F-63AED2010B8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{32CBE812-E37C-4690-A61F-63AED2010B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="ranking_metadados" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="183">
   <si>
     <t>4.2.1</t>
   </si>
@@ -304,9 +304,6 @@
     <t>MT0014794891.mp3</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>100 FEATURES COSSENO</t>
   </si>
   <si>
@@ -590,6 +587,18 @@
   </si>
   <si>
     <t>Column21</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>desvio padrao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desvio padrao </t>
+  </si>
+  <si>
+    <t xml:space="preserve">media </t>
   </si>
 </sst>
 </file>
@@ -668,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -681,11 +690,224 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -796,27 +1018,27 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A368D4E-E194-4B2D-ACC9-D1329352AE5C}" name="ranking_metadados" displayName="ranking_metadados" ref="A1:U5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:U5" xr:uid="{8A368D4E-E194-4B2D-ACC9-D1329352AE5C}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{FA5D10F0-1118-4830-8F53-78C9C23976AA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{4CBF984B-899C-4C89-8393-090AE58CC05F}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{F8FCA89C-960B-4EC7-A0AF-8048655E7535}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{A4D9B129-E534-40F3-8174-D7B2DA6D45B5}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{1C3662AD-A7F4-46A1-AC2E-14E12A86FB94}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{97847BA1-32F8-497A-86E7-F87768C695BE}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{405CD2D5-D9D7-4474-83C4-A9ADD7CEBAD6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{B36A12C8-906D-44D7-B7A9-3912B3B2C68E}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{FBD7EEC2-E9E3-46A8-975D-F4878EF0E756}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{C5E0223D-39F8-46CD-A003-D1DE38988E2B}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{86420E36-BC95-4160-A038-3B80850181DD}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{6CB7DC69-08CA-480E-AAC4-CD351CEB9C0F}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{62366952-0071-4EEC-925C-6BB688C423FF}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{1C4E126F-F2B1-4CE2-A57F-03E646AC6AE8}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{DC7288F9-12D0-4969-9190-09B29B8EA1F3}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{0D97A783-02F9-495B-9B6C-70B9B0C68B52}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{3A1CFEC4-5EF4-4DB4-A75C-CACEEC7E9D06}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{324979EC-C20B-4D95-B9CE-E7F592AE21C5}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{347E1D6E-592E-48F3-B6CC-7E65A1241D65}" uniqueName="19" name="Column19" queryTableFieldId="19" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{327587FB-F2C7-4B3D-A4AD-66A206F93BB1}" uniqueName="20" name="Column20" queryTableFieldId="20" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{8FFC355F-6C8C-4DE9-8151-5D4BA714730E}" uniqueName="21" name="Column21" queryTableFieldId="21" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FA5D10F0-1118-4830-8F53-78C9C23976AA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{4CBF984B-899C-4C89-8393-090AE58CC05F}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{F8FCA89C-960B-4EC7-A0AF-8048655E7535}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{A4D9B129-E534-40F3-8174-D7B2DA6D45B5}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{1C3662AD-A7F4-46A1-AC2E-14E12A86FB94}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{97847BA1-32F8-497A-86E7-F87768C695BE}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{405CD2D5-D9D7-4474-83C4-A9ADD7CEBAD6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{B36A12C8-906D-44D7-B7A9-3912B3B2C68E}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{FBD7EEC2-E9E3-46A8-975D-F4878EF0E756}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{C5E0223D-39F8-46CD-A003-D1DE38988E2B}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{86420E36-BC95-4160-A038-3B80850181DD}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{6CB7DC69-08CA-480E-AAC4-CD351CEB9C0F}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{62366952-0071-4EEC-925C-6BB688C423FF}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{1C4E126F-F2B1-4CE2-A57F-03E646AC6AE8}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{DC7288F9-12D0-4969-9190-09B29B8EA1F3}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{0D97A783-02F9-495B-9B6C-70B9B0C68B52}" uniqueName="16" name="Column16" queryTableFieldId="16" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{3A1CFEC4-5EF4-4DB4-A75C-CACEEC7E9D06}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{324979EC-C20B-4D95-B9CE-E7F592AE21C5}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{347E1D6E-592E-48F3-B6CC-7E65A1241D65}" uniqueName="19" name="Column19" queryTableFieldId="19" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{327587FB-F2C7-4B3D-A4AD-66A206F93BB1}" uniqueName="20" name="Column20" queryTableFieldId="20" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{8FFC355F-6C8C-4DE9-8151-5D4BA714730E}" uniqueName="21" name="Column21" queryTableFieldId="21" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1123,334 +1345,334 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="21" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
         <v>159</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>160</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>161</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>162</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>163</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>164</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>165</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>166</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>167</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>168</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>169</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>170</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>171</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>172</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>173</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>175</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>176</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>177</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>178</v>
       </c>
-      <c r="U1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>50</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="U2" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="T3" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="U3" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="U3" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>60</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="L4" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="N4" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="O4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="P4" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q4" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="R4" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="S4" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="T4" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="T4" s="11" t="s">
+      <c r="U4" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="U4" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>77</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="N5" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="R5" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>157</v>
       </c>
       <c r="T5" s="11" t="s">
         <v>72</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1463,66 +1685,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81AFAB82-1159-4B26-9158-54B42BE2DE54}">
-  <dimension ref="A1:O117"/>
+  <dimension ref="A1:Q119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" t="s">
         <v>85</v>
       </c>
-      <c r="N3" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>182</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="N4" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f>AVERAGE(C6:D6)</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="O5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="O6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>AVERAGE(C7:D7)</f>
         <v>1</v>
       </c>
       <c r="N7" s="8" t="s">
@@ -1532,572 +1771,908 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>84</v>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(C8:D8)</f>
+        <v>1.5</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f>AVERAGE(C9:D9)</f>
+        <v>2</v>
+      </c>
       <c r="N9" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>AVERAGE(C10:D10)</f>
+        <v>1</v>
+      </c>
       <c r="N10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <f>AVERAGE(C11:D11)</f>
+        <v>3</v>
+      </c>
       <c r="N11" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f>AVERAGE(C12:D12)</f>
+        <v>1</v>
+      </c>
       <c r="N12" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(C13:D13)</f>
+        <v>5</v>
+      </c>
       <c r="N13" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f>AVERAGE(C14:D14)</f>
+        <v>1.5</v>
+      </c>
       <c r="N14" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(C15:D15)</f>
+        <v>4</v>
+      </c>
       <c r="N15" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f>AVERAGE(C16:D16)</f>
+        <v>1.5</v>
+      </c>
       <c r="N16" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGE(C17:D17)</f>
+        <v>2.5</v>
+      </c>
       <c r="N17" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f>AVERAGE(C18:D18)</f>
+        <v>1</v>
+      </c>
       <c r="N18" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <f>AVERAGE(C19:D19)</f>
+        <v>2.5</v>
+      </c>
       <c r="N19" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <f>AVERAGE(C20:D20)</f>
+        <v>3.5</v>
+      </c>
       <c r="N20" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f>AVERAGE(C21:D21)</f>
+        <v>3.5</v>
+      </c>
       <c r="N21" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f>AVERAGE(C22:D22)</f>
+        <v>1</v>
+      </c>
       <c r="N22" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGE(C23:D23)</f>
+        <v>2.5</v>
+      </c>
       <c r="N23" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGE(C24:D24)</f>
+        <v>1</v>
+      </c>
       <c r="N24" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <f>AVERAGE(C25:D25)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26">
+        <f>AVERAGE(C6:C25)</f>
+        <v>1.95</v>
+      </c>
+      <c r="D26">
+        <f>AVERAGE(D6:D25)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q26" s="14"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27">
+        <f>STDEV(C6:C25)</f>
+        <v>1.2763022245616642</v>
+      </c>
+      <c r="D27">
+        <f>STDEV(D6:D25)</f>
+        <v>1.1742858972247996</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E39" t="s">
+        <v>179</v>
+      </c>
       <c r="N39" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <f>AVERAGE(C40:D40)</f>
+        <v>2</v>
+      </c>
       <c r="N40" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <f>AVERAGE(C41:D41)</f>
+        <v>2.5</v>
+      </c>
       <c r="N41" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O41">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <f>AVERAGE(C42:D42)</f>
+        <v>1</v>
+      </c>
       <c r="N42" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C43">
         <v>4</v>
       </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <f>AVERAGE(C43:D43)</f>
+        <v>4</v>
+      </c>
       <c r="N43" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <f>AVERAGE(C44:D44)</f>
+        <v>1.5</v>
+      </c>
       <c r="N44" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <f>AVERAGE(C45:D45)</f>
+        <v>3</v>
+      </c>
       <c r="N45" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O45">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <f>AVERAGE(C46:D46)</f>
+        <v>2.5</v>
+      </c>
       <c r="N46" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f>AVERAGE(C47:D47)</f>
+        <v>1</v>
+      </c>
       <c r="N47" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O47">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <f>AVERAGE(C48:D48)</f>
+        <v>1.5</v>
+      </c>
       <c r="N48" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O48">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <f>AVERAGE(C49:D49)</f>
+        <v>2.5</v>
+      </c>
       <c r="N49" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O49">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <f>AVERAGE(C50:D50)</f>
+        <v>2</v>
+      </c>
       <c r="N50" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <f>AVERAGE(C51:D51)</f>
+        <v>1</v>
+      </c>
       <c r="N51" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O51">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C52">
         <v>2</v>
       </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <f>AVERAGE(C52:D52)</f>
+        <v>2.5</v>
+      </c>
       <c r="N52" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O52">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <f>AVERAGE(C53:D53)</f>
+        <v>1</v>
+      </c>
       <c r="N53" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O53">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <f>AVERAGE(C54:D54)</f>
+        <v>2</v>
+      </c>
       <c r="N54" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <f>AVERAGE(C55:D55)</f>
+        <v>1.5</v>
+      </c>
       <c r="N55" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O55">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <f>AVERAGE(C56:D56)</f>
+        <v>1</v>
+      </c>
       <c r="N56" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57">
+        <f>AVERAGE(C57:D57)</f>
+        <v>2.5</v>
+      </c>
       <c r="N57" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <f>AVERAGE(C58:D58)</f>
+        <v>1</v>
+      </c>
       <c r="N58" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O58">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <f>AVERAGE(C59:D59)</f>
+        <v>2</v>
+      </c>
       <c r="N59" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O59">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60">
+        <f>AVERAGE(C40:C59)</f>
+        <v>1.7</v>
+      </c>
+      <c r="D60">
+        <f>AVERAGE(D40:D59)</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61">
+        <f>STDEV(C40:C59)</f>
+        <v>0.86450472587061755</v>
+      </c>
+      <c r="D61">
+        <f>STDEV(D40:D59)</f>
+        <v>1.0208355710680808</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
         <v>43</v>
       </c>
+      <c r="E70" t="s">
+        <v>179</v>
+      </c>
       <c r="N70" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C71">
         <v>3</v>
       </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <f>AVERAGE(C71:D71)</f>
+        <v>2.5</v>
+      </c>
       <c r="N71" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O71">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <f>AVERAGE(C72:D72)</f>
+        <v>2</v>
+      </c>
       <c r="N72" s="8" t="s">
         <v>58</v>
       </c>
@@ -2105,27 +2680,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <f>AVERAGE(C73:D73)</f>
+        <v>1</v>
+      </c>
       <c r="N73" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O73">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B74" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <f>AVERAGE(C74:D74)</f>
+        <v>1</v>
+      </c>
       <c r="N74" s="8" t="s">
         <v>60</v>
       </c>
@@ -2133,83 +2722,125 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <f>AVERAGE(C75:D75)</f>
+        <v>1</v>
+      </c>
       <c r="N75" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O75">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <f>AVERAGE(C76:D76)</f>
+        <v>1</v>
+      </c>
       <c r="N76" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O76">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <f>AVERAGE(C77:D77)</f>
+        <v>1.5</v>
+      </c>
       <c r="N77" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O77">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C78">
         <v>2</v>
       </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <f>AVERAGE(C78:D78)</f>
+        <v>1.5</v>
+      </c>
       <c r="N78" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O78">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C79">
         <v>3</v>
       </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+      <c r="E79">
+        <f>AVERAGE(C79:D79)</f>
+        <v>3</v>
+      </c>
       <c r="N79" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C80">
         <v>2</v>
       </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <f>AVERAGE(C80:D80)</f>
+        <v>2.5</v>
+      </c>
       <c r="N80" s="8" t="s">
         <v>41</v>
       </c>
@@ -2217,55 +2848,83 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <f>AVERAGE(C81:D81)</f>
+        <v>1</v>
+      </c>
       <c r="N81" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O81">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <f>AVERAGE(C82:D82)</f>
+        <v>1.5</v>
+      </c>
       <c r="N82" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <f>AVERAGE(C83:D83)</f>
+        <v>1</v>
+      </c>
       <c r="N83" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <f>AVERAGE(C84:D84)</f>
+        <v>1</v>
+      </c>
       <c r="N84" s="8" t="s">
         <v>25</v>
       </c>
@@ -2273,119 +2932,204 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C85">
         <v>5</v>
       </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85">
+        <f>AVERAGE(C85:D85)</f>
+        <v>4.5</v>
+      </c>
       <c r="N85" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O85">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86">
+        <f>AVERAGE(C86:D86)</f>
+        <v>1.5</v>
+      </c>
       <c r="N86" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O86">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C87">
         <v>5</v>
       </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87">
+        <f>AVERAGE(C87:D87)</f>
+        <v>5</v>
+      </c>
       <c r="N87" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O87">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C88">
         <v>3</v>
       </c>
+      <c r="D88">
+        <v>4</v>
+      </c>
+      <c r="E88">
+        <f>AVERAGE(C88:D88)</f>
+        <v>3.5</v>
+      </c>
       <c r="N88" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O88">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <f>AVERAGE(C89:D89)</f>
+        <v>1.5</v>
+      </c>
       <c r="N89" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O89">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C90">
         <v>2</v>
       </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+      <c r="E90">
+        <f>AVERAGE(C90:D90)</f>
+        <v>2.5</v>
+      </c>
       <c r="N90" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O90">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B91" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C91">
+        <f>AVERAGE(C71:C90)</f>
+        <v>1.85</v>
+      </c>
+      <c r="D91">
+        <f>AVERAGE(D71:D90)</f>
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B92" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C92">
+        <f>STDEV(C71:C90)</f>
+        <v>1.3088765773505315</v>
+      </c>
+      <c r="D92">
+        <f>STDEV(D71:D90)</f>
+        <v>1.2258187382102494</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="E97" t="s">
+        <v>179</v>
+      </c>
       <c r="N97" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C98">
         <v>4</v>
       </c>
+      <c r="D98">
+        <v>5</v>
+      </c>
+      <c r="E98">
+        <f>AVERAGE(C98:D98)</f>
+        <v>4.5</v>
+      </c>
       <c r="N98" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O98">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C99">
         <v>3</v>
       </c>
+      <c r="D99">
+        <v>5</v>
+      </c>
+      <c r="E99">
+        <f>AVERAGE(C99:D99)</f>
+        <v>4</v>
+      </c>
       <c r="N99" s="5" t="s">
         <v>68</v>
       </c>
@@ -2393,27 +3137,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C100">
         <v>3</v>
       </c>
+      <c r="D100">
+        <v>5</v>
+      </c>
+      <c r="E100">
+        <f>AVERAGE(C100:D100)</f>
+        <v>4</v>
+      </c>
       <c r="N100" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O100">
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
+      <c r="D101">
+        <v>4</v>
+      </c>
+      <c r="E101">
+        <f>AVERAGE(C101:D101)</f>
+        <v>3</v>
+      </c>
+      <c r="K101" s="14"/>
       <c r="N101" s="5" t="s">
         <v>77</v>
       </c>
@@ -2421,209 +3180,314 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C102">
         <v>5</v>
       </c>
+      <c r="D102">
+        <v>4</v>
+      </c>
+      <c r="E102">
+        <f>AVERAGE(C102:D102)</f>
+        <v>4.5</v>
+      </c>
       <c r="N102" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O102">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103">
+        <f>AVERAGE(C103:D103)</f>
+        <v>1</v>
+      </c>
       <c r="N103" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O103">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C104">
         <v>3</v>
       </c>
+      <c r="D104">
+        <v>4</v>
+      </c>
+      <c r="E104">
+        <f>AVERAGE(C104:D104)</f>
+        <v>3.5</v>
+      </c>
       <c r="N104" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O104">
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+      <c r="E105">
+        <f>AVERAGE(C105:D105)</f>
+        <v>2</v>
+      </c>
       <c r="N105" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O105">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
+      <c r="D106">
+        <v>3</v>
+      </c>
+      <c r="E106">
+        <f>AVERAGE(C106:D106)</f>
+        <v>2</v>
+      </c>
       <c r="N106" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O106">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <f>AVERAGE(C107:D107)</f>
+        <v>1</v>
+      </c>
       <c r="N107" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O107">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
+      <c r="D108">
+        <v>2</v>
+      </c>
+      <c r="E108">
+        <f>AVERAGE(C108:D108)</f>
+        <v>1.5</v>
+      </c>
       <c r="N108" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O108">
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <f>AVERAGE(C109:D109)</f>
+        <v>1</v>
+      </c>
       <c r="N109" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O109">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <f>AVERAGE(C110:D110)</f>
+        <v>1</v>
+      </c>
       <c r="N110" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O110">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
+      <c r="D111">
+        <v>4</v>
+      </c>
+      <c r="E111">
+        <f>AVERAGE(C111:D111)</f>
+        <v>2.5</v>
+      </c>
       <c r="N111" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O111">
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <f>AVERAGE(C112:D112)</f>
+        <v>1</v>
+      </c>
       <c r="N112" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O112">
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+      <c r="E113">
+        <f>AVERAGE(C113:D113)</f>
+        <v>1.5</v>
+      </c>
       <c r="N113" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O113">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B114" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+      <c r="E114">
+        <f>AVERAGE(C114:D114)</f>
+        <v>2</v>
+      </c>
       <c r="N114" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O114">
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C115" s="5">
         <v>4</v>
       </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115">
+        <f>AVERAGE(C115:D115)</f>
+        <v>3.5</v>
+      </c>
       <c r="N115" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O115">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C116" s="10">
         <v>2</v>
       </c>
+      <c r="D116">
+        <v>3</v>
+      </c>
+      <c r="E116">
+        <f>AVERAGE(C116:D116)</f>
+        <v>2.5</v>
+      </c>
       <c r="N116" s="5" t="s">
         <v>72</v>
       </c>
@@ -2631,22 +3495,82 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B117" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C117" s="10">
         <v>2</v>
       </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
+      <c r="E117">
+        <f>AVERAGE(C117:D117)</f>
+        <v>2</v>
+      </c>
       <c r="N117" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O117">
         <v>5</v>
       </c>
     </row>
+    <row r="118" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B118" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C118">
+        <f>AVERAGE(C98:C117)</f>
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <f>AVERAGE(D98:D117)</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="119" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B119" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C119">
+        <f>STDEV(C98:C117)</f>
+        <v>1.2565617248750864</v>
+      </c>
+      <c r="D119">
+        <f>STDEV(D98:D117)</f>
+        <v>1.4363696929192156</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="E40:E59">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="greaterThan">
+      <formula>"2.4"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+      <formula>2.4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:E25">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+      <formula>2.4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71:E90">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+      <formula>"2.4"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+      <formula>2.4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E98:E117">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>2.4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>